<commit_message>
A bunch of changes. Three general sets. First is to cleanup the process of generating the nutrient lookup table. This is not yet complete. The second is to change the file naming convention to use underscore rather than period so sweave (which uses latex) can be used. Finally the ODBC script to read in nutrient data was split in two and also integrated with the dataPrep.nutrients script.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/NutrientCodeLookup.xlsx
+++ b/data-raw/NutrientData/NutrientCodeLookup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -32,9 +32,6 @@
     <t>Nutr_No</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>Tagname</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>nutCode</t>
+  </si>
+  <si>
+    <t>unit</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,16 +646,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -663,16 +663,16 @@
         <v>262</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -680,16 +680,16 @@
         <v>301</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -697,16 +697,16 @@
         <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -714,16 +714,16 @@
         <v>601</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>54</v>
       </c>
-      <c r="D5" t="s">
-        <v>55</v>
-      </c>
       <c r="E5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -731,16 +731,16 @@
         <v>208</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -748,16 +748,16 @@
         <v>645</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
         <v>58</v>
       </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
       <c r="E7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -765,16 +765,16 @@
         <v>646</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s">
         <v>60</v>
       </c>
-      <c r="D8" t="s">
-        <v>61</v>
-      </c>
       <c r="E8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -782,16 +782,16 @@
         <v>606</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -799,16 +799,16 @@
         <v>291</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -816,16 +816,16 @@
         <v>435</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -833,16 +833,16 @@
         <v>303</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
       <c r="E12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -850,16 +850,16 @@
         <v>304</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" t="s">
-        <v>24</v>
-      </c>
       <c r="E13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -867,16 +867,16 @@
         <v>406</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
         <v>44</v>
       </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -884,16 +884,16 @@
         <v>305</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -901,16 +901,16 @@
         <v>306</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
       <c r="E16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -918,16 +918,16 @@
         <v>203</v>
       </c>
       <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
         <v>4</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>5</v>
       </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -935,16 +935,16 @@
         <v>405</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" t="s">
-        <v>43</v>
-      </c>
       <c r="E18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -952,16 +952,16 @@
         <v>404</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
         <v>40</v>
       </c>
-      <c r="D19" t="s">
-        <v>41</v>
-      </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -969,16 +969,16 @@
         <v>204</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
         <v>7</v>
       </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
       <c r="E20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -986,16 +986,16 @@
         <v>320</v>
       </c>
       <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
-        <v>33</v>
-      </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1003,16 +1003,16 @@
         <v>418</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
         <v>48</v>
       </c>
-      <c r="D22" t="s">
-        <v>49</v>
-      </c>
       <c r="E22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1020,16 +1020,16 @@
         <v>415</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
-        <v>47</v>
-      </c>
       <c r="E23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1037,16 +1037,16 @@
         <v>401</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
         <v>38</v>
       </c>
-      <c r="D24" t="s">
-        <v>39</v>
-      </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1054,16 +1054,16 @@
         <v>328</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
         <v>36</v>
       </c>
-      <c r="D25" t="s">
-        <v>37</v>
-      </c>
       <c r="E25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1071,16 +1071,16 @@
         <v>323</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" t="s">
         <v>34</v>
       </c>
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1088,16 +1088,16 @@
         <v>430</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
         <v>50</v>
       </c>
-      <c r="D27" t="s">
-        <v>51</v>
-      </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1105,16 +1105,16 @@
         <v>309</v>
       </c>
       <c r="B28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" t="s">
         <v>29</v>
       </c>
-      <c r="D28" t="s">
-        <v>30</v>
-      </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1122,16 +1122,16 @@
         <v>269</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" t="s">
         <v>91</v>
       </c>
-      <c r="D29" t="s">
-        <v>92</v>
-      </c>
       <c r="E29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1139,16 +1139,16 @@
         <v>605</v>
       </c>
       <c r="B30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
         <v>93</v>
       </c>
-      <c r="D30" t="s">
-        <v>94</v>
-      </c>
       <c r="E30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Many changes to deal with phytate issues.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/NutrientCodeLookup.xlsx
+++ b/data-raw/NutrientData/NutrientCodeLookup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -632,7 +632,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
A bunch of code cleanup including fixing elasticity bug, file name changes, etc.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/NutrientCodeLookup.xlsx
+++ b/data-raw/NutrientData/NutrientCodeLookup.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-29100" yWindow="-4940" windowWidth="27360" windowHeight="14860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27360" windowHeight="14860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="nutr_def" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="99">
   <si>
     <t>Nutr_No</t>
   </si>
@@ -315,19 +315,33 @@
   </si>
   <si>
     <t>unit</t>
+  </si>
+  <si>
+    <t>ethanol_g</t>
+  </si>
+  <si>
+    <t>Alcohol, ethyl</t>
+  </si>
+  <si>
+    <t>ALC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Sans"/>
     </font>
   </fonts>
   <fills count="2">
@@ -350,8 +364,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E30"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1151,6 +1166,23 @@
         <v>89</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>221</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E31" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="E16:E48">
     <sortCondition ref="E15"/>

</xml_diff>

<commit_message>
a bunch of fixes to get ready for final version
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/NutrientCodeLookup.xlsx
+++ b/data-raw/NutrientData/NutrientCodeLookup.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB86630-7A0B-5E40-B1F6-CB98FA904DAA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27360" windowHeight="14860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27360" windowHeight="14860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nutr_def" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
   <si>
     <t>Nutr_No</t>
   </si>
@@ -324,12 +325,66 @@
   </si>
   <si>
     <t>ALC</t>
+  </si>
+  <si>
+    <t>NutrShortDesc</t>
+  </si>
+  <si>
+    <t>Carbohydrate</t>
+  </si>
+  <si>
+    <t>Folate</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Magnesium</t>
+  </si>
+  <si>
+    <t>Phosphorus</t>
+  </si>
+  <si>
+    <t>Potassium</t>
+  </si>
+  <si>
+    <t>Vitamin B12</t>
+  </si>
+  <si>
+    <t>Vitamin B6</t>
+  </si>
+  <si>
+    <t>Vitamin C</t>
+  </si>
+  <si>
+    <t>Vitamin D</t>
+  </si>
+  <si>
+    <t>Vitamin E</t>
+  </si>
+  <si>
+    <t>Vitamin K</t>
+  </si>
+  <si>
+    <t>Zinc</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>Alcohol</t>
+  </si>
+  <si>
+    <t>Calcium</t>
+  </si>
+  <si>
+    <t>Vitamin A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -376,6 +431,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -643,11 +701,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -656,7 +714,7 @@
     <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -672,8 +730,11 @@
       <c r="E1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>262</v>
       </c>
@@ -689,8 +750,11 @@
       <c r="E2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>301</v>
       </c>
@@ -706,8 +770,11 @@
       <c r="E3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>205</v>
       </c>
@@ -723,8 +790,11 @@
       <c r="E4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>601</v>
       </c>
@@ -740,8 +810,11 @@
       <c r="E5" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>208</v>
       </c>
@@ -757,8 +830,11 @@
       <c r="E6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>645</v>
       </c>
@@ -774,8 +850,11 @@
       <c r="E7" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>646</v>
       </c>
@@ -791,8 +870,11 @@
       <c r="E8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>606</v>
       </c>
@@ -808,8 +890,11 @@
       <c r="E9" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>291</v>
       </c>
@@ -825,8 +910,11 @@
       <c r="E10" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>435</v>
       </c>
@@ -842,8 +930,11 @@
       <c r="E11" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>303</v>
       </c>
@@ -859,8 +950,11 @@
       <c r="E12" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>304</v>
       </c>
@@ -876,8 +970,11 @@
       <c r="E13" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>406</v>
       </c>
@@ -893,8 +990,11 @@
       <c r="E14" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>305</v>
       </c>
@@ -910,8 +1010,11 @@
       <c r="E15" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>306</v>
       </c>
@@ -927,8 +1030,11 @@
       <c r="E16" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>203</v>
       </c>
@@ -944,8 +1050,11 @@
       <c r="E17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>405</v>
       </c>
@@ -961,8 +1070,11 @@
       <c r="E18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>404</v>
       </c>
@@ -978,8 +1090,11 @@
       <c r="E19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>204</v>
       </c>
@@ -995,8 +1110,11 @@
       <c r="E20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>320</v>
       </c>
@@ -1012,8 +1130,11 @@
       <c r="E21" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>418</v>
       </c>
@@ -1029,8 +1150,11 @@
       <c r="E22" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>415</v>
       </c>
@@ -1046,8 +1170,11 @@
       <c r="E23" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>401</v>
       </c>
@@ -1063,8 +1190,11 @@
       <c r="E24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>328</v>
       </c>
@@ -1080,8 +1210,11 @@
       <c r="E25" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>323</v>
       </c>
@@ -1097,8 +1230,11 @@
       <c r="E26" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>430</v>
       </c>
@@ -1114,8 +1250,11 @@
       <c r="E27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>309</v>
       </c>
@@ -1131,8 +1270,11 @@
       <c r="E28" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>269</v>
       </c>
@@ -1148,8 +1290,11 @@
       <c r="E29" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>605</v>
       </c>
@@ -1165,8 +1310,11 @@
       <c r="E30" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>221</v>
       </c>
@@ -1181,6 +1329,9 @@
       </c>
       <c r="E31" t="s">
         <v>96</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various changes in preparation for final nutrient modeling paper.
</commit_message>
<xml_diff>
--- a/data-raw/NutrientData/NutrientCodeLookup.xlsx
+++ b/data-raw/NutrientData/NutrientCodeLookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11104"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutmod/data-raw/NutrientData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB86630-7A0B-5E40-B1F6-CB98FA904DAA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6221A81-F551-3D4C-9EB4-99794858322F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27360" windowHeight="14860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34100" yWindow="-1880" windowWidth="27360" windowHeight="14860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nutr_def" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="119">
   <si>
     <t>Nutr_No</t>
   </si>
@@ -379,6 +379,12 @@
   </si>
   <si>
     <t>Vitamin A</t>
+  </si>
+  <si>
+    <t>phytate_mg</t>
+  </si>
+  <si>
+    <t>Phytate</t>
   </si>
 </sst>
 </file>
@@ -397,6 +403,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Lucida Sans"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -702,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1334,6 +1341,20 @@
         <v>114</v>
       </c>
     </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" t="s">
+        <v>118</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="E16:E48">
     <sortCondition ref="E15"/>

</xml_diff>